<commit_message>
change dob type template excel
</commit_message>
<xml_diff>
--- a/src/services/excel/templates/import-nurse-template.xlsx
+++ b/src/services/excel/templates/import-nurse-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\SchoolMedix_BE\src\services\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B833CC-1E08-4EF7-BAE7-FE4D7CB4CA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8144DEEA-A6FF-4559-8FCC-BCD661B9EA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Nguyễn Văn A</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Nguyễn Văn C</t>
   </si>
   <si>
-    <t>14/03/2000</t>
-  </si>
-  <si>
-    <t>20/11/1993</t>
-  </si>
-  <si>
     <t>0362718422</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
   </si>
   <si>
     <t>Trần Thị D</t>
-  </si>
-  <si>
-    <t>20/11/1990</t>
   </si>
   <si>
     <t>asdffd@gmail.com</t>
@@ -125,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -173,9 +164,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -184,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -469,37 +460,37 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12" style="6" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="J1"/>
       <c r="K1"/>
@@ -514,34 +505,34 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
+      <c r="C2" s="6">
+        <v>32479</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="C3" s="6">
+        <v>32479</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -551,102 +542,102 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>32479</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>32479</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
+      <c r="A6" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>32479</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="6">
+        <v>32479</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="6">
+        <v>32479</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="5"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>